<commit_message>
Merged PR 7638: PRI-23411 Quarter without Guaranteed Demo with only ADUs displays empty Guaranteed Demo table
PRI-23411 Implementation and tests
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractTypeWithRestrictions.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/Campaign export/CampaignExport_ContractTypeWithRestrictions.xlsx
@@ -981,7 +981,7 @@
     <t>Broadcast Proposal Campaign with all types of plans</t>
   </si>
   <si>
-    <t>Created 02/27/20</t>
+    <t>Created 02/28/20</t>
   </si>
   <si>
     <t>Stub Agency</t>
@@ -2578,7 +2578,7 @@
       </c>
       <c r="L2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/27/20</v>
+        <v>Created 02/28/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>
@@ -6669,7 +6669,7 @@
       <c r="K2" s="5"/>
       <c r="P2" s="6" t="str">
         <f>'PROPOSAL'!T2</f>
-        <v>Created 02/27/20</v>
+        <v>Created 02/28/20</v>
       </c>
     </row>
     <row r="3" ht="18" customHeight="1"/>

</xml_diff>